<commit_message>
lots of little tweaks
</commit_message>
<xml_diff>
--- a/build/data/maindata.xlsx
+++ b/build/data/maindata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hargaja/Desktop/workspace/elections/20180927-absentee/build/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A96672-E354-1949-9F11-0BC8EAD9C385}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03C142C-EA51-7841-B4EA-5B88225B472A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="460" windowWidth="26900" windowHeight="17360" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5300" yWindow="1040" windowWidth="26900" windowHeight="17360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018age" sheetId="11" r:id="rId1"/>
@@ -10911,8 +10911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34709779-4AE9-184C-8747-61ED2F71A71A}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15554,8 +15554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P32" sqref="P32:P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>